<commit_message>
multi entity final and dynamic
</commit_message>
<xml_diff>
--- a/Documents/MultiEntity.xlsx
+++ b/Documents/MultiEntity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Others\SF-Test\DocumentPocGit\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCABD366-87D5-463C-9A66-169EDFCFC17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A70F49E-0A1A-4166-B9C5-8F443F346A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B11E4CF4-4A34-4901-ACAB-97798AB95730}"/>
   </bookViews>
@@ -441,7 +441,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>